<commit_message>
Weekly backup - October 19, 2017
</commit_message>
<xml_diff>
--- a/wp-content/uploads/Ratecard-AdUX.xlsx
+++ b/wp-content/uploads/Ratecard-AdUX.xlsx
@@ -5,11 +5,11 @@
   <workbookPr updateLinks="never" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannane\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christelle\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="7680" tabRatio="830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16785" windowHeight="7305" tabRatio="830"/>
   </bookViews>
   <sheets>
     <sheet name="General Conditions" sheetId="22" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="338">
   <si>
     <t>Marmiton</t>
   </si>
@@ -1008,6 +1008,69 @@
     <t>mgenot@adux.com</t>
   </si>
   <si>
+    <t>CPP</t>
+  </si>
+  <si>
+    <t>Pack Sliding video*</t>
+  </si>
+  <si>
+    <t>*100% SOV</t>
+  </si>
+  <si>
+    <t>CPM 50€</t>
+  </si>
+  <si>
+    <t>CPM 40€</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>Auto &amp; News</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Food &amp; Drink</t>
+  </si>
+  <si>
+    <t>Large format**</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Via Michelin</t>
+  </si>
+  <si>
+    <t>from 5.000€</t>
+  </si>
+  <si>
+    <t>Openingsuren/Heures-d'Ouvertures</t>
+  </si>
+  <si>
+    <t>In-Banner video</t>
+  </si>
+  <si>
+    <t>Lesly Bakkaus</t>
+  </si>
+  <si>
+    <t>Marketing &amp; Publisher Executive</t>
+  </si>
+  <si>
+    <t>lbakkaus@adux.com</t>
+  </si>
+  <si>
+    <t>02/894 84 03</t>
+  </si>
+  <si>
+    <t>adpulsebe@adux.com</t>
+  </si>
+  <si>
+    <t>doc.adux.be</t>
+  </si>
+  <si>
+    <t>Click to download</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">General Conditions
 </t>
@@ -1022,71 +1085,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Q3 2017</t>
+      <t>Q4 2017</t>
     </r>
-  </si>
-  <si>
-    <t>CPP</t>
-  </si>
-  <si>
-    <t>Pack Sliding video*</t>
-  </si>
-  <si>
-    <t>*100% SOV</t>
-  </si>
-  <si>
-    <t>CPM 50€</t>
-  </si>
-  <si>
-    <t>CPM 40€</t>
-  </si>
-  <si>
-    <t>Pack</t>
-  </si>
-  <si>
-    <t>Auto &amp; News</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Food &amp; Drink</t>
-  </si>
-  <si>
-    <t>Large format**</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Via Michelin</t>
-  </si>
-  <si>
-    <t>from 5.000€</t>
-  </si>
-  <si>
-    <t>Openingsuren/Heures-d'Ouvertures</t>
-  </si>
-  <si>
-    <t>In-Banner video</t>
-  </si>
-  <si>
-    <t>Lesly Bakkaus</t>
-  </si>
-  <si>
-    <t>Marketing &amp; Publisher Executive</t>
-  </si>
-  <si>
-    <t>lbakkaus@adux.com</t>
-  </si>
-  <si>
-    <t>02/894 84 03</t>
-  </si>
-  <si>
-    <t>adpulsebe@adux.com</t>
-  </si>
-  <si>
-    <t>doc.adux.be</t>
-  </si>
-  <si>
-    <t>Click to download</t>
   </si>
 </sst>
 </file>
@@ -1094,25 +1094,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="19">
-    <numFmt numFmtId="8" formatCode="&quot;€&quot;\ #,##0.00;[Red]&quot;€&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="&quot;€&quot;\ #,##0_-"/>
-    <numFmt numFmtId="169" formatCode="&quot;€&quot;\ #,##0.00_-"/>
-    <numFmt numFmtId="170" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="172" formatCode="0.0%"/>
-    <numFmt numFmtId="173" formatCode="_-* #,##0.00&quot; €&quot;_-;\-* #,##0.00&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
-    <numFmt numFmtId="174" formatCode="&quot;€&quot;\ #,##0"/>
-    <numFmt numFmtId="175" formatCode="_([$€-2]* #,##0.0_);_([$€-2]* \(#,##0.0\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="176" formatCode="_([$€-2]* #,##0_);_([$€-2]* \(#,##0\);_([$€-2]* &quot;-&quot;??_)"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00\ [$€-40C];\-#,##0.00\ [$€-40C]"/>
-    <numFmt numFmtId="178" formatCode="#,##0\ [$€-40C];\-#,##0\ [$€-40C]"/>
-    <numFmt numFmtId="179" formatCode="#,##0_ ;\-#,##0\ "/>
-    <numFmt numFmtId="180" formatCode="##\ &quot;€&quot;"/>
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00;[Red]&quot;€&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="&quot;€&quot;\ #,##0_-"/>
+    <numFmt numFmtId="167" formatCode="&quot;€&quot;\ #,##0.00_-"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_([$€-2]* #,##0.00_);_([$€-2]* \(#,##0.00\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0.00&quot; €&quot;_-;\-* #,##0.00&quot; €&quot;_-;_-* \-??&quot; €&quot;_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="&quot;€&quot;\ #,##0"/>
+    <numFmt numFmtId="173" formatCode="_([$€-2]* #,##0.0_);_([$€-2]* \(#,##0.0\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="174" formatCode="_([$€-2]* #,##0_);_([$€-2]* \(#,##0\);_([$€-2]* &quot;-&quot;??_)"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00\ [$€-40C];\-#,##0.00\ [$€-40C]"/>
+    <numFmt numFmtId="176" formatCode="#,##0\ [$€-40C];\-#,##0\ [$€-40C]"/>
+    <numFmt numFmtId="177" formatCode="#,##0_ ;\-#,##0\ "/>
+    <numFmt numFmtId="178" formatCode="##\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="44" x14ac:knownFonts="1">
     <font>
@@ -2782,47 +2782,47 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="12" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -2868,9 +2868,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2882,9 +2882,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -2895,9 +2895,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2907,9 +2907,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2919,9 +2919,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2931,9 +2931,9 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -2941,40 +2941,40 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="341">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2996,15 +2996,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="10" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="18" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="10" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="18" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="10" fillId="9" borderId="0" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="18" fillId="9" borderId="0" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="18" fillId="9" borderId="0" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="18" fillId="9" borderId="0" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="9" fontId="18" fillId="9" borderId="0" xfId="272" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3021,10 +3021,10 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="9" borderId="0" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="0" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="18" fillId="9" borderId="18" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="18" fillId="9" borderId="18" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="18" fillId="9" borderId="18" xfId="272" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3033,7 +3033,7 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="18" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="15" fillId="9" borderId="18" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="9" borderId="18" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3044,19 +3044,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3" readingOrder="1"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="9" borderId="28" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="28" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="2" borderId="30" xfId="361" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="24" fillId="2" borderId="30" xfId="361" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3086,35 +3086,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="10" fillId="9" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="32" fillId="8" borderId="18" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="10" fillId="9" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="32" fillId="8" borderId="18" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="9" fillId="9" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="9" fillId="9" borderId="25" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="9" fillId="9" borderId="26" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="9" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="9" fillId="9" borderId="27" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="18" fillId="9" borderId="29" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="10" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="9" fillId="9" borderId="0" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="9" fillId="9" borderId="25" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="9" fillId="9" borderId="26" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="9" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="9" fillId="9" borderId="27" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="18" fillId="9" borderId="29" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="10" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="18" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="18" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="33" fillId="9" borderId="28" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="28" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="36" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="10" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="38" fillId="9" borderId="27" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="10" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="38" fillId="9" borderId="27" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="9" borderId="18" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="18" fillId="9" borderId="18" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="10" fillId="9" borderId="44" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="10" fillId="9" borderId="44" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -3128,13 +3128,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="26" xfId="262" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="15" fillId="9" borderId="25" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="15" fillId="9" borderId="25" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="25" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="18" fillId="9" borderId="25" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="10" fillId="9" borderId="25" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="10" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="18" fillId="9" borderId="25" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="10" fillId="9" borderId="25" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="10" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="26" xfId="300" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="26" xfId="362" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="26" xfId="261" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3148,7 +3148,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3166,16 +3166,16 @@
     <xf numFmtId="0" fontId="39" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="39" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3191,16 +3191,16 @@
     <xf numFmtId="3" fontId="26" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="3" xfId="363" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="3" xfId="363" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="6" xfId="363" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="6" xfId="363" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="64" xfId="363" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="64" xfId="363" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="65" xfId="363" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="65" xfId="363" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="8" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3221,7 +3221,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3250,22 +3250,22 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="9" fillId="9" borderId="22" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="9" fillId="9" borderId="23" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="9" fillId="9" borderId="24" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="9" fillId="9" borderId="22" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="9" fillId="9" borderId="23" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="9" fillId="9" borderId="24" xfId="238" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="7" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="41" fillId="8" borderId="71" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="41" fillId="8" borderId="71" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="41" fillId="8" borderId="73" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="41" fillId="8" borderId="73" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="41" fillId="8" borderId="72" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="41" fillId="8" borderId="72" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3296,17 +3296,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3348,10 +3348,10 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3376,7 +3376,7 @@
     <xf numFmtId="3" fontId="7" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="41" fillId="8" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="41" fillId="8" borderId="30" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3427,27 +3427,66 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="27" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="28" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="29" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="9" borderId="18" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="9" borderId="0" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="9" borderId="26" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="25" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="26" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="56" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="57" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="9" borderId="25" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="40" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="17" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="15" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="57" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3496,48 +3535,12 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="9" borderId="27" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="9" borderId="28" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="9" borderId="29" xfId="260" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="9" borderId="18" xfId="272" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="15" fillId="9" borderId="0" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="15" fillId="9" borderId="26" xfId="261" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="25" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="26" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="25" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="40" fillId="9" borderId="26" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3547,36 +3550,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3589,6 +3589,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3601,25 +3613,19 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="6" fillId="8" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="6" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="6" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3640,77 +3646,77 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="26" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="174" fontId="26" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -3718,9 +3724,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="8" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3730,7 +3733,10 @@
     <xf numFmtId="3" fontId="7" fillId="8" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="42" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="59" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="51" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3739,11 +3745,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="60" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="59" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3763,13 +3775,10 @@
     <xf numFmtId="0" fontId="22" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="33" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="33" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="37" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="9" borderId="0" xfId="238" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="40" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3809,15 +3818,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4258,7 +4258,7 @@
         <xdr:cNvPr id="2" name="Image 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4337,7 +4337,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="Résultat de recherche d'images pour &quot;microsoft nouveau logo png&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6456,7 +6456,7 @@
         <xdr:cNvPr id="6" name="Image 5" descr="Résultat de recherche d'images pour &quot;microsoft nouveau logo png&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7657,7 +7657,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F865116-8830-43AB-B730-E43892058C40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2F865116-8830-43AB-B730-E43892058C40}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -12824,7 +12824,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="Résultat de recherche d'images pour &quot;microsoft nouveau logo png&quot;">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13557,8 +13557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13572,84 +13572,84 @@
   <sheetData>
     <row r="1" spans="2:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="217"/>
-      <c r="C2" s="220" t="s">
-        <v>316</v>
-      </c>
-      <c r="D2" s="220"/>
-      <c r="E2" s="220"/>
-      <c r="F2" s="220"/>
-      <c r="G2" s="220"/>
-      <c r="H2" s="221"/>
+      <c r="B2" s="230"/>
+      <c r="C2" s="233" t="s">
+        <v>337</v>
+      </c>
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
+      <c r="F2" s="233"/>
+      <c r="G2" s="233"/>
+      <c r="H2" s="234"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="218"/>
-      <c r="C3" s="222"/>
-      <c r="D3" s="222"/>
-      <c r="E3" s="222"/>
-      <c r="F3" s="222"/>
-      <c r="G3" s="222"/>
-      <c r="H3" s="223"/>
+      <c r="B3" s="231"/>
+      <c r="C3" s="235"/>
+      <c r="D3" s="235"/>
+      <c r="E3" s="235"/>
+      <c r="F3" s="235"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="236"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="218"/>
-      <c r="C4" s="222"/>
-      <c r="D4" s="222"/>
-      <c r="E4" s="222"/>
-      <c r="F4" s="222"/>
-      <c r="G4" s="222"/>
-      <c r="H4" s="223"/>
+      <c r="B4" s="231"/>
+      <c r="C4" s="235"/>
+      <c r="D4" s="235"/>
+      <c r="E4" s="235"/>
+      <c r="F4" s="235"/>
+      <c r="G4" s="235"/>
+      <c r="H4" s="236"/>
     </row>
     <row r="5" spans="2:8" ht="78" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="219"/>
-      <c r="C5" s="224"/>
-      <c r="D5" s="224"/>
-      <c r="E5" s="224"/>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="225"/>
+      <c r="B5" s="232"/>
+      <c r="C5" s="237"/>
+      <c r="D5" s="237"/>
+      <c r="E5" s="237"/>
+      <c r="F5" s="237"/>
+      <c r="G5" s="237"/>
+      <c r="H5" s="238"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="226"/>
-      <c r="C6" s="227"/>
-      <c r="D6" s="227"/>
-      <c r="E6" s="227"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="227"/>
-      <c r="H6" s="228"/>
+      <c r="B6" s="239"/>
+      <c r="C6" s="240"/>
+      <c r="D6" s="240"/>
+      <c r="E6" s="240"/>
+      <c r="F6" s="240"/>
+      <c r="G6" s="240"/>
+      <c r="H6" s="241"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="212" t="s">
+      <c r="B7" s="221" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="215"/>
-      <c r="D7" s="215"/>
-      <c r="E7" s="215"/>
-      <c r="F7" s="215"/>
-      <c r="G7" s="215"/>
-      <c r="H7" s="216"/>
+      <c r="C7" s="223"/>
+      <c r="D7" s="223"/>
+      <c r="E7" s="223"/>
+      <c r="F7" s="223"/>
+      <c r="G7" s="223"/>
+      <c r="H7" s="224"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="229"/>
-      <c r="C8" s="230"/>
-      <c r="D8" s="231"/>
-      <c r="E8" s="230"/>
-      <c r="F8" s="230"/>
-      <c r="G8" s="230"/>
-      <c r="H8" s="232"/>
+      <c r="B8" s="242"/>
+      <c r="C8" s="243"/>
+      <c r="D8" s="244"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="243"/>
+      <c r="G8" s="243"/>
+      <c r="H8" s="245"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="212" t="s">
+      <c r="B9" s="221" t="s">
         <v>256</v>
       </c>
-      <c r="C9" s="213"/>
+      <c r="C9" s="228"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="214" t="s">
+      <c r="E9" s="229" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="215"/>
-      <c r="G9" s="215"/>
-      <c r="H9" s="216"/>
+      <c r="F9" s="223"/>
+      <c r="G9" s="223"/>
+      <c r="H9" s="224"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="74"/>
@@ -13668,10 +13668,10 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D11" s="15"/>
-      <c r="E11" s="236" t="s">
+      <c r="E11" s="215" t="s">
         <v>135</v>
       </c>
-      <c r="F11" s="236"/>
+      <c r="F11" s="215"/>
       <c r="G11" s="175" t="s">
         <v>56</v>
       </c>
@@ -13685,10 +13685,10 @@
         <v>0.05</v>
       </c>
       <c r="D12" s="16"/>
-      <c r="E12" s="236" t="s">
+      <c r="E12" s="215" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="236"/>
+      <c r="F12" s="215"/>
       <c r="G12" s="175">
         <v>0.25</v>
       </c>
@@ -13702,10 +13702,10 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="D13" s="15"/>
-      <c r="E13" s="236" t="s">
+      <c r="E13" s="215" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="236"/>
+      <c r="F13" s="215"/>
       <c r="G13" s="175">
         <v>0.25</v>
       </c>
@@ -13719,10 +13719,10 @@
         <v>0.1</v>
       </c>
       <c r="D14" s="16"/>
-      <c r="E14" s="236" t="s">
+      <c r="E14" s="215" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="236"/>
+      <c r="F14" s="215"/>
       <c r="G14" s="175">
         <v>0.5</v>
       </c>
@@ -13736,10 +13736,10 @@
         <v>0.125</v>
       </c>
       <c r="D15" s="15"/>
-      <c r="E15" s="236" t="s">
+      <c r="E15" s="215" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="236"/>
+      <c r="F15" s="215"/>
       <c r="G15" s="175">
         <v>0.15</v>
       </c>
@@ -13781,12 +13781,12 @@
         <v>0.2</v>
       </c>
       <c r="D18" s="16"/>
-      <c r="E18" s="237" t="s">
+      <c r="E18" s="216" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="237"/>
-      <c r="G18" s="237"/>
-      <c r="H18" s="238"/>
+      <c r="F18" s="216"/>
+      <c r="G18" s="216"/>
+      <c r="H18" s="217"/>
     </row>
     <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="30" t="s">
@@ -13796,10 +13796,10 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="D19" s="15"/>
-      <c r="E19" s="237"/>
-      <c r="F19" s="237"/>
-      <c r="G19" s="237"/>
-      <c r="H19" s="238"/>
+      <c r="E19" s="216"/>
+      <c r="F19" s="216"/>
+      <c r="G19" s="216"/>
+      <c r="H19" s="217"/>
     </row>
     <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="30" t="s">
@@ -13848,15 +13848,15 @@
       <c r="H23" s="76"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="239" t="s">
+      <c r="B24" s="218" t="s">
         <v>218</v>
       </c>
-      <c r="C24" s="240"/>
-      <c r="D24" s="240"/>
-      <c r="E24" s="240"/>
-      <c r="F24" s="240"/>
-      <c r="G24" s="240"/>
-      <c r="H24" s="241"/>
+      <c r="C24" s="219"/>
+      <c r="D24" s="219"/>
+      <c r="E24" s="219"/>
+      <c r="F24" s="219"/>
+      <c r="G24" s="219"/>
+      <c r="H24" s="220"/>
     </row>
     <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="78"/>
@@ -13922,15 +13922,15 @@
       <c r="H29" s="76"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="212" t="s">
+      <c r="B30" s="221" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="242"/>
-      <c r="D30" s="215"/>
-      <c r="E30" s="242"/>
-      <c r="F30" s="215"/>
-      <c r="G30" s="215"/>
-      <c r="H30" s="216"/>
+      <c r="C30" s="222"/>
+      <c r="D30" s="223"/>
+      <c r="E30" s="222"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="223"/>
+      <c r="H30" s="224"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="80"/>
@@ -13942,15 +13942,15 @@
       <c r="H31" s="81"/>
     </row>
     <row r="32" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="243" t="s">
+      <c r="B32" s="225" t="s">
         <v>290</v>
       </c>
-      <c r="C32" s="244"/>
-      <c r="D32" s="244"/>
-      <c r="E32" s="244"/>
-      <c r="F32" s="244"/>
-      <c r="G32" s="244"/>
-      <c r="H32" s="245"/>
+      <c r="C32" s="226"/>
+      <c r="D32" s="226"/>
+      <c r="E32" s="226"/>
+      <c r="F32" s="226"/>
+      <c r="G32" s="226"/>
+      <c r="H32" s="227"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="80"/>
@@ -14184,17 +14184,17 @@
     </row>
     <row r="47" spans="2:8" s="182" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="79" t="s">
+        <v>330</v>
+      </c>
+      <c r="C47" s="12" t="s">
         <v>331</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>332</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="F47" s="21" t="s">
         <v>333</v>
-      </c>
-      <c r="F47" s="21" t="s">
-        <v>334</v>
       </c>
       <c r="G47" s="22"/>
       <c r="H47" s="82"/>
@@ -14277,15 +14277,15 @@
       <c r="H52" s="81"/>
     </row>
     <row r="53" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="243" t="s">
+      <c r="B53" s="225" t="s">
         <v>91</v>
       </c>
-      <c r="C53" s="244"/>
-      <c r="D53" s="244"/>
-      <c r="E53" s="244"/>
-      <c r="F53" s="244"/>
-      <c r="G53" s="244"/>
-      <c r="H53" s="245"/>
+      <c r="C53" s="226"/>
+      <c r="D53" s="226"/>
+      <c r="E53" s="226"/>
+      <c r="F53" s="226"/>
+      <c r="G53" s="226"/>
+      <c r="H53" s="227"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="80"/>
@@ -14353,7 +14353,7 @@
         <v>96</v>
       </c>
       <c r="C59" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D59" s="24"/>
       <c r="E59" s="17"/>
@@ -14384,15 +14384,15 @@
       <c r="H61" s="81"/>
     </row>
     <row r="62" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B62" s="243" t="s">
+      <c r="B62" s="225" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="244"/>
-      <c r="D62" s="244"/>
-      <c r="E62" s="244"/>
-      <c r="F62" s="244"/>
-      <c r="G62" s="244"/>
-      <c r="H62" s="245"/>
+      <c r="C62" s="226"/>
+      <c r="D62" s="226"/>
+      <c r="E62" s="226"/>
+      <c r="F62" s="226"/>
+      <c r="G62" s="226"/>
+      <c r="H62" s="227"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="80"/>
@@ -14504,7 +14504,7 @@
         <v>105</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D72" s="24"/>
       <c r="E72" s="22"/>
@@ -14517,7 +14517,7 @@
         <v>42</v>
       </c>
       <c r="C73" s="20" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D73" s="24"/>
       <c r="E73" s="22"/>
@@ -14577,18 +14577,25 @@
       <c r="H78" s="89"/>
     </row>
     <row r="79" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="233" t="s">
+      <c r="B79" s="212" t="s">
         <v>167</v>
       </c>
-      <c r="C79" s="234"/>
-      <c r="D79" s="234"/>
-      <c r="E79" s="234"/>
-      <c r="F79" s="234"/>
-      <c r="G79" s="234"/>
-      <c r="H79" s="235"/>
+      <c r="C79" s="213"/>
+      <c r="D79" s="213"/>
+      <c r="E79" s="213"/>
+      <c r="F79" s="213"/>
+      <c r="G79" s="213"/>
+      <c r="H79" s="214"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B8:H8"/>
     <mergeCell ref="B79:H79"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E12:F12"/>
@@ -14601,13 +14608,6 @@
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="B53:H53"/>
     <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B8:H8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C55" r:id="rId1"/>
@@ -14709,47 +14709,47 @@
     </row>
     <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="34"/>
-      <c r="C8" s="305"/>
+      <c r="C8" s="307"/>
       <c r="D8" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="305"/>
+      <c r="E8" s="307"/>
       <c r="F8" s="35"/>
     </row>
     <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="34"/>
-      <c r="C9" s="306"/>
+      <c r="C9" s="308"/>
       <c r="D9" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="306"/>
+      <c r="E9" s="308"/>
       <c r="F9" s="35"/>
     </row>
     <row r="10" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="34"/>
-      <c r="C10" s="306"/>
+      <c r="C10" s="308"/>
       <c r="D10" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="E10" s="306"/>
+      <c r="E10" s="308"/>
       <c r="F10" s="35"/>
     </row>
     <row r="11" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="34"/>
-      <c r="C11" s="306"/>
+      <c r="C11" s="308"/>
       <c r="D11" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="E11" s="306"/>
+      <c r="E11" s="308"/>
       <c r="F11" s="35"/>
     </row>
     <row r="12" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="34"/>
-      <c r="C12" s="307"/>
+      <c r="C12" s="306"/>
       <c r="D12" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="E12" s="307"/>
+      <c r="E12" s="306"/>
       <c r="F12" s="35"/>
     </row>
     <row r="13" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -14761,24 +14761,24 @@
     </row>
     <row r="14" spans="2:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="34"/>
-      <c r="C14" s="308" t="s">
+      <c r="C14" s="309" t="s">
         <v>261</v>
       </c>
-      <c r="D14" s="309"/>
-      <c r="E14" s="310"/>
+      <c r="D14" s="310"/>
+      <c r="E14" s="311"/>
       <c r="F14" s="35"/>
     </row>
     <row r="15" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="34"/>
-      <c r="C15" s="311"/>
-      <c r="D15" s="311"/>
+      <c r="C15" s="305"/>
+      <c r="D15" s="305"/>
       <c r="E15" s="118"/>
       <c r="F15" s="35"/>
     </row>
     <row r="16" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34"/>
-      <c r="C16" s="307"/>
-      <c r="D16" s="307"/>
+      <c r="C16" s="306"/>
+      <c r="D16" s="306"/>
       <c r="E16" s="119"/>
       <c r="F16" s="35"/>
     </row>
@@ -14797,15 +14797,15 @@
     </row>
     <row r="18" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="34"/>
-      <c r="C18" s="311"/>
-      <c r="D18" s="311"/>
+      <c r="C18" s="305"/>
+      <c r="D18" s="305"/>
       <c r="E18" s="118"/>
       <c r="F18" s="35"/>
     </row>
     <row r="19" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="34"/>
-      <c r="C19" s="307"/>
-      <c r="D19" s="307"/>
+      <c r="C19" s="306"/>
+      <c r="D19" s="306"/>
       <c r="E19" s="119"/>
       <c r="F19" s="35"/>
     </row>
@@ -14824,15 +14824,15 @@
     </row>
     <row r="21" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="34"/>
-      <c r="C21" s="311"/>
-      <c r="D21" s="311"/>
+      <c r="C21" s="305"/>
+      <c r="D21" s="305"/>
       <c r="E21" s="118"/>
       <c r="F21" s="35"/>
     </row>
     <row r="22" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="34"/>
-      <c r="C22" s="307"/>
-      <c r="D22" s="307"/>
+      <c r="C22" s="306"/>
+      <c r="D22" s="306"/>
       <c r="E22" s="119"/>
       <c r="F22" s="35"/>
     </row>
@@ -14909,27 +14909,27 @@
     </row>
     <row r="30" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="36"/>
-      <c r="C30" s="255" t="s">
+      <c r="C30" s="251" t="s">
         <v>215</v>
       </c>
-      <c r="D30" s="255"/>
-      <c r="E30" s="255"/>
-      <c r="F30" s="256"/>
+      <c r="D30" s="251"/>
+      <c r="E30" s="251"/>
+      <c r="F30" s="252"/>
       <c r="G30" s="3"/>
       <c r="H30" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="C30:F30"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
@@ -15008,22 +15008,22 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="34"/>
-      <c r="C7" s="314"/>
-      <c r="D7" s="311"/>
-      <c r="E7" s="311"/>
-      <c r="F7" s="311"/>
-      <c r="G7" s="311"/>
-      <c r="H7" s="312"/>
+      <c r="C7" s="312"/>
+      <c r="D7" s="305"/>
+      <c r="E7" s="305"/>
+      <c r="F7" s="305"/>
+      <c r="G7" s="305"/>
+      <c r="H7" s="314"/>
       <c r="I7" s="35"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="34"/>
-      <c r="C8" s="315"/>
-      <c r="D8" s="307"/>
-      <c r="E8" s="307"/>
-      <c r="F8" s="307"/>
-      <c r="G8" s="307"/>
-      <c r="H8" s="313"/>
+      <c r="C8" s="313"/>
+      <c r="D8" s="306"/>
+      <c r="E8" s="306"/>
+      <c r="F8" s="306"/>
+      <c r="G8" s="306"/>
+      <c r="H8" s="315"/>
       <c r="I8" s="35"/>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15060,22 +15060,22 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="34"/>
-      <c r="C11" s="314"/>
-      <c r="D11" s="311"/>
-      <c r="E11" s="311"/>
-      <c r="F11" s="311"/>
-      <c r="G11" s="311"/>
-      <c r="H11" s="312"/>
+      <c r="C11" s="312"/>
+      <c r="D11" s="305"/>
+      <c r="E11" s="305"/>
+      <c r="F11" s="305"/>
+      <c r="G11" s="305"/>
+      <c r="H11" s="314"/>
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="34"/>
-      <c r="C12" s="315"/>
-      <c r="D12" s="307"/>
-      <c r="E12" s="307"/>
-      <c r="F12" s="307"/>
-      <c r="G12" s="307"/>
-      <c r="H12" s="313"/>
+      <c r="C12" s="313"/>
+      <c r="D12" s="306"/>
+      <c r="E12" s="306"/>
+      <c r="F12" s="306"/>
+      <c r="G12" s="306"/>
+      <c r="H12" s="315"/>
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15112,22 +15112,22 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="34"/>
-      <c r="C15" s="314"/>
-      <c r="D15" s="311"/>
-      <c r="E15" s="311"/>
-      <c r="F15" s="311"/>
-      <c r="G15" s="311"/>
-      <c r="H15" s="312"/>
+      <c r="C15" s="312"/>
+      <c r="D15" s="305"/>
+      <c r="E15" s="305"/>
+      <c r="F15" s="305"/>
+      <c r="G15" s="305"/>
+      <c r="H15" s="314"/>
       <c r="I15" s="35"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="34"/>
-      <c r="C16" s="315"/>
-      <c r="D16" s="307"/>
-      <c r="E16" s="307"/>
-      <c r="F16" s="307"/>
-      <c r="G16" s="307"/>
-      <c r="H16" s="313"/>
+      <c r="C16" s="313"/>
+      <c r="D16" s="306"/>
+      <c r="E16" s="306"/>
+      <c r="F16" s="306"/>
+      <c r="G16" s="306"/>
+      <c r="H16" s="315"/>
       <c r="I16" s="35"/>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15164,22 +15164,22 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="34"/>
-      <c r="C19" s="314"/>
-      <c r="D19" s="311"/>
-      <c r="E19" s="311"/>
-      <c r="F19" s="311"/>
-      <c r="G19" s="311"/>
-      <c r="H19" s="312"/>
+      <c r="C19" s="312"/>
+      <c r="D19" s="305"/>
+      <c r="E19" s="305"/>
+      <c r="F19" s="305"/>
+      <c r="G19" s="305"/>
+      <c r="H19" s="314"/>
       <c r="I19" s="35"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="34"/>
-      <c r="C20" s="315"/>
-      <c r="D20" s="307"/>
-      <c r="E20" s="307"/>
-      <c r="F20" s="307"/>
-      <c r="G20" s="307"/>
-      <c r="H20" s="313"/>
+      <c r="C20" s="313"/>
+      <c r="D20" s="306"/>
+      <c r="E20" s="306"/>
+      <c r="F20" s="306"/>
+      <c r="G20" s="306"/>
+      <c r="H20" s="315"/>
       <c r="I20" s="35"/>
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15253,31 +15253,15 @@
       <c r="C26" s="93"/>
       <c r="D26" s="93"/>
       <c r="E26" s="93"/>
-      <c r="F26" s="255" t="s">
+      <c r="F26" s="251" t="s">
         <v>167</v>
       </c>
-      <c r="G26" s="255"/>
-      <c r="H26" s="255"/>
-      <c r="I26" s="256"/>
+      <c r="G26" s="251"/>
+      <c r="H26" s="251"/>
+      <c r="I26" s="252"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="G19:G20"/>
@@ -15287,6 +15271,22 @@
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15324,22 +15324,22 @@
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="59"/>
-      <c r="C3" s="316" t="s">
+      <c r="C3" s="320" t="s">
         <v>298</v>
       </c>
-      <c r="D3" s="317"/>
-      <c r="E3" s="317"/>
-      <c r="F3" s="317"/>
-      <c r="G3" s="318"/>
+      <c r="D3" s="321"/>
+      <c r="E3" s="321"/>
+      <c r="F3" s="321"/>
+      <c r="G3" s="322"/>
       <c r="H3" s="60"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="59"/>
-      <c r="C4" s="319"/>
-      <c r="D4" s="320"/>
-      <c r="E4" s="320"/>
-      <c r="F4" s="320"/>
-      <c r="G4" s="321"/>
+      <c r="C4" s="323"/>
+      <c r="D4" s="324"/>
+      <c r="E4" s="324"/>
+      <c r="F4" s="324"/>
+      <c r="G4" s="325"/>
       <c r="H4" s="60"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -15362,10 +15362,10 @@
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="59"/>
-      <c r="C7" s="336" t="s">
+      <c r="C7" s="339" t="s">
         <v>240</v>
       </c>
-      <c r="D7" s="337"/>
+      <c r="D7" s="340"/>
       <c r="E7" s="57" t="s">
         <v>236</v>
       </c>
@@ -15379,66 +15379,66 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="59"/>
-      <c r="C8" s="327"/>
-      <c r="D8" s="330"/>
-      <c r="E8" s="332" t="s">
+      <c r="C8" s="330"/>
+      <c r="D8" s="333"/>
+      <c r="E8" s="335" t="s">
         <v>239</v>
       </c>
-      <c r="F8" s="332" t="s">
+      <c r="F8" s="335" t="s">
         <v>246</v>
       </c>
-      <c r="G8" s="338">
+      <c r="G8" s="316">
         <v>1.63</v>
       </c>
       <c r="H8" s="60"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="59"/>
-      <c r="C9" s="328"/>
-      <c r="D9" s="331"/>
-      <c r="E9" s="333"/>
-      <c r="F9" s="333"/>
-      <c r="G9" s="339"/>
+      <c r="C9" s="331"/>
+      <c r="D9" s="334"/>
+      <c r="E9" s="336"/>
+      <c r="F9" s="336"/>
+      <c r="G9" s="317"/>
       <c r="H9" s="60"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="59"/>
-      <c r="C10" s="328"/>
-      <c r="D10" s="331"/>
-      <c r="E10" s="334"/>
-      <c r="F10" s="334"/>
-      <c r="G10" s="339"/>
+      <c r="C10" s="331"/>
+      <c r="D10" s="334"/>
+      <c r="E10" s="337"/>
+      <c r="F10" s="337"/>
+      <c r="G10" s="317"/>
       <c r="H10" s="60"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="59"/>
-      <c r="C11" s="328"/>
-      <c r="D11" s="331"/>
-      <c r="E11" s="333" t="s">
+      <c r="C11" s="331"/>
+      <c r="D11" s="334"/>
+      <c r="E11" s="336" t="s">
         <v>238</v>
       </c>
-      <c r="F11" s="333" t="s">
+      <c r="F11" s="336" t="s">
         <v>247</v>
       </c>
-      <c r="G11" s="339"/>
+      <c r="G11" s="317"/>
       <c r="H11" s="60"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="59"/>
-      <c r="C12" s="328"/>
-      <c r="D12" s="331"/>
-      <c r="E12" s="333"/>
-      <c r="F12" s="333"/>
-      <c r="G12" s="339"/>
+      <c r="C12" s="331"/>
+      <c r="D12" s="334"/>
+      <c r="E12" s="336"/>
+      <c r="F12" s="336"/>
+      <c r="G12" s="317"/>
       <c r="H12" s="60"/>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="59"/>
-      <c r="C13" s="329"/>
+      <c r="C13" s="332"/>
       <c r="D13" s="171"/>
-      <c r="E13" s="335"/>
-      <c r="F13" s="335"/>
-      <c r="G13" s="340"/>
+      <c r="E13" s="338"/>
+      <c r="F13" s="338"/>
+      <c r="G13" s="318"/>
       <c r="H13" s="60"/>
     </row>
     <row r="14" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15452,13 +15452,13 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="59"/>
-      <c r="C15" s="325" t="s">
+      <c r="C15" s="328" t="s">
         <v>142</v>
       </c>
-      <c r="D15" s="326"/>
-      <c r="E15" s="326"/>
-      <c r="F15" s="326"/>
-      <c r="G15" s="326"/>
+      <c r="D15" s="329"/>
+      <c r="E15" s="329"/>
+      <c r="F15" s="329"/>
+      <c r="G15" s="329"/>
       <c r="H15" s="60"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -15472,123 +15472,123 @@
     </row>
     <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="59"/>
-      <c r="C17" s="322" t="s">
+      <c r="C17" s="326" t="s">
         <v>241</v>
       </c>
-      <c r="D17" s="322"/>
-      <c r="E17" s="322"/>
-      <c r="F17" s="322"/>
-      <c r="G17" s="322"/>
+      <c r="D17" s="326"/>
+      <c r="E17" s="326"/>
+      <c r="F17" s="326"/>
+      <c r="G17" s="326"/>
       <c r="H17" s="61"/>
     </row>
     <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="59"/>
-      <c r="C18" s="323" t="s">
+      <c r="C18" s="319" t="s">
         <v>172</v>
       </c>
-      <c r="D18" s="323"/>
-      <c r="E18" s="323"/>
-      <c r="F18" s="323"/>
-      <c r="G18" s="323"/>
+      <c r="D18" s="319"/>
+      <c r="E18" s="319"/>
+      <c r="F18" s="319"/>
+      <c r="G18" s="319"/>
       <c r="H18" s="61"/>
     </row>
     <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="59"/>
-      <c r="C19" s="323" t="s">
+      <c r="C19" s="319" t="s">
         <v>252</v>
       </c>
-      <c r="D19" s="323"/>
-      <c r="E19" s="323"/>
-      <c r="F19" s="323"/>
-      <c r="G19" s="323"/>
+      <c r="D19" s="319"/>
+      <c r="E19" s="319"/>
+      <c r="F19" s="319"/>
+      <c r="G19" s="319"/>
       <c r="H19" s="61"/>
     </row>
     <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="59"/>
-      <c r="C20" s="323" t="s">
+      <c r="C20" s="319" t="s">
         <v>219</v>
       </c>
-      <c r="D20" s="323"/>
-      <c r="E20" s="323"/>
-      <c r="F20" s="323"/>
-      <c r="G20" s="323"/>
+      <c r="D20" s="319"/>
+      <c r="E20" s="319"/>
+      <c r="F20" s="319"/>
+      <c r="G20" s="319"/>
       <c r="H20" s="61"/>
     </row>
     <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="59"/>
-      <c r="C21" s="323" t="s">
+      <c r="C21" s="319" t="s">
         <v>220</v>
       </c>
-      <c r="D21" s="323"/>
-      <c r="E21" s="323"/>
-      <c r="F21" s="323"/>
-      <c r="G21" s="323"/>
+      <c r="D21" s="319"/>
+      <c r="E21" s="319"/>
+      <c r="F21" s="319"/>
+      <c r="G21" s="319"/>
       <c r="H21" s="61"/>
     </row>
     <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="59"/>
-      <c r="C22" s="323" t="s">
+      <c r="C22" s="319" t="s">
         <v>221</v>
       </c>
-      <c r="D22" s="323"/>
-      <c r="E22" s="323"/>
-      <c r="F22" s="323"/>
-      <c r="G22" s="323"/>
+      <c r="D22" s="319"/>
+      <c r="E22" s="319"/>
+      <c r="F22" s="319"/>
+      <c r="G22" s="319"/>
       <c r="H22" s="61"/>
     </row>
     <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="59"/>
-      <c r="C23" s="322" t="s">
+      <c r="C23" s="326" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="322"/>
-      <c r="E23" s="322"/>
-      <c r="F23" s="322"/>
-      <c r="G23" s="322"/>
+      <c r="D23" s="326"/>
+      <c r="E23" s="326"/>
+      <c r="F23" s="326"/>
+      <c r="G23" s="326"/>
       <c r="H23" s="61"/>
     </row>
     <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="59"/>
-      <c r="C24" s="323" t="s">
+      <c r="C24" s="319" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="323"/>
-      <c r="E24" s="323"/>
-      <c r="F24" s="323"/>
-      <c r="G24" s="323"/>
+      <c r="D24" s="319"/>
+      <c r="E24" s="319"/>
+      <c r="F24" s="319"/>
+      <c r="G24" s="319"/>
       <c r="H24" s="61"/>
     </row>
     <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="59"/>
-      <c r="C25" s="324" t="s">
+      <c r="C25" s="327" t="s">
         <v>171</v>
       </c>
-      <c r="D25" s="324"/>
-      <c r="E25" s="324"/>
-      <c r="F25" s="324"/>
-      <c r="G25" s="324"/>
+      <c r="D25" s="327"/>
+      <c r="E25" s="327"/>
+      <c r="F25" s="327"/>
+      <c r="G25" s="327"/>
       <c r="H25" s="64"/>
     </row>
     <row r="26" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="59"/>
-      <c r="C26" s="324" t="s">
+      <c r="C26" s="327" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="324"/>
-      <c r="E26" s="324"/>
-      <c r="F26" s="324"/>
-      <c r="G26" s="324"/>
+      <c r="D26" s="327"/>
+      <c r="E26" s="327"/>
+      <c r="F26" s="327"/>
+      <c r="G26" s="327"/>
       <c r="H26" s="64"/>
     </row>
     <row r="27" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="59"/>
-      <c r="C27" s="323" t="s">
+      <c r="C27" s="319" t="s">
         <v>299</v>
       </c>
-      <c r="D27" s="323"/>
-      <c r="E27" s="323"/>
-      <c r="F27" s="323"/>
-      <c r="G27" s="323"/>
+      <c r="D27" s="319"/>
+      <c r="E27" s="319"/>
+      <c r="F27" s="319"/>
+      <c r="G27" s="319"/>
       <c r="H27" s="65"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15602,12 +15602,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="C24:G24"/>
@@ -15624,6 +15618,12 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F11:F13"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15636,7 +15636,7 @@
   <dimension ref="B1:P27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15682,8 +15682,8 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="250"/>
-      <c r="G4" s="250"/>
+      <c r="F4" s="253"/>
+      <c r="G4" s="253"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -15703,18 +15703,18 @@
     </row>
     <row r="6" spans="2:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="34"/>
-      <c r="C6" s="253" t="s">
+      <c r="C6" s="255" t="s">
         <v>257</v>
       </c>
-      <c r="D6" s="253"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="253"/>
-      <c r="G6" s="254"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="256"/>
       <c r="H6" s="114" t="s">
         <v>300</v>
       </c>
       <c r="I6" s="115" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J6" s="116" t="s">
         <v>231</v>
@@ -15723,10 +15723,10 @@
     </row>
     <row r="7" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="34"/>
-      <c r="C7" s="251" t="s">
+      <c r="C7" s="254" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="251"/>
+      <c r="D7" s="254"/>
       <c r="E7" s="136" t="s">
         <v>7</v>
       </c>
@@ -15749,10 +15749,10 @@
     </row>
     <row r="8" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="34"/>
-      <c r="C8" s="252" t="s">
+      <c r="C8" s="247" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="252"/>
+      <c r="D8" s="247"/>
       <c r="E8" s="246" t="s">
         <v>182</v>
       </c>
@@ -15767,16 +15767,16 @@
         <v>800000</v>
       </c>
       <c r="J8" s="192">
-        <v>447043</v>
+        <v>200000</v>
       </c>
       <c r="K8" s="35"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="34"/>
-      <c r="C9" s="252" t="s">
+      <c r="C9" s="247" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="252"/>
+      <c r="D9" s="247"/>
       <c r="E9" s="246" t="s">
         <v>182</v>
       </c>
@@ -15791,17 +15791,17 @@
         <v>900000</v>
       </c>
       <c r="J9" s="192">
-        <v>358478</v>
+        <v>600000</v>
       </c>
       <c r="K9" s="35"/>
       <c r="P9" s="173"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="34"/>
-      <c r="C10" s="247" t="s">
+      <c r="C10" s="248" t="s">
         <v>251</v>
       </c>
-      <c r="D10" s="247"/>
+      <c r="D10" s="248"/>
       <c r="E10" s="209">
         <v>0.85</v>
       </c>
@@ -15841,17 +15841,17 @@
       <c r="I11" s="192">
         <v>1000000</v>
       </c>
-      <c r="J11" s="192" t="s">
-        <v>12</v>
+      <c r="J11" s="192">
+        <v>500000</v>
       </c>
       <c r="K11" s="35"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="34"/>
-      <c r="C12" s="248" t="s">
-        <v>329</v>
-      </c>
-      <c r="D12" s="249"/>
+      <c r="C12" s="249" t="s">
+        <v>328</v>
+      </c>
+      <c r="D12" s="250"/>
       <c r="E12" s="209">
         <v>0.2</v>
       </c>
@@ -15892,16 +15892,16 @@
         <v>700000</v>
       </c>
       <c r="J13" s="192">
-        <v>70120</v>
+        <v>1100000</v>
       </c>
       <c r="K13" s="35"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="34"/>
-      <c r="C14" s="248" t="s">
+      <c r="C14" s="249" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="249"/>
+      <c r="D14" s="250"/>
       <c r="E14" s="246" t="s">
         <v>182</v>
       </c>
@@ -15916,16 +15916,16 @@
         <v>1600000</v>
       </c>
       <c r="J14" s="192">
-        <v>548849</v>
+        <v>350000</v>
       </c>
       <c r="K14" s="35"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="34"/>
-      <c r="C15" s="252" t="s">
+      <c r="C15" s="247" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="252"/>
+      <c r="D15" s="247"/>
       <c r="E15" s="246" t="s">
         <v>182</v>
       </c>
@@ -15940,17 +15940,17 @@
         <v>350000</v>
       </c>
       <c r="J15" s="192">
-        <v>246438</v>
+        <v>1200000</v>
       </c>
       <c r="K15" s="35"/>
       <c r="P15" s="173"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="34"/>
-      <c r="C16" s="252" t="s">
+      <c r="C16" s="247" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="252"/>
+      <c r="D16" s="247"/>
       <c r="E16" s="246" t="s">
         <v>182</v>
       </c>
@@ -15965,16 +15965,16 @@
         <v>2200000</v>
       </c>
       <c r="J16" s="192">
-        <v>278851</v>
+        <v>100000</v>
       </c>
       <c r="K16" s="35"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="34"/>
-      <c r="C17" s="247" t="s">
+      <c r="C17" s="248" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="247"/>
+      <c r="D17" s="248"/>
       <c r="E17" s="209">
         <v>0.7</v>
       </c>
@@ -15997,10 +15997,10 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="34"/>
-      <c r="C18" s="252" t="s">
-        <v>327</v>
-      </c>
-      <c r="D18" s="252"/>
+      <c r="C18" s="247" t="s">
+        <v>326</v>
+      </c>
+      <c r="D18" s="247"/>
       <c r="E18" s="209">
         <v>0.7</v>
       </c>
@@ -16023,10 +16023,10 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="34"/>
-      <c r="C19" s="247" t="s">
+      <c r="C19" s="248" t="s">
         <v>297</v>
       </c>
-      <c r="D19" s="247"/>
+      <c r="D19" s="248"/>
       <c r="E19" s="209">
         <v>0.3</v>
       </c>
@@ -16049,10 +16049,10 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="34"/>
-      <c r="C20" s="247" t="s">
+      <c r="C20" s="248" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="247"/>
+      <c r="D20" s="248"/>
       <c r="E20" s="209">
         <v>0.47</v>
       </c>
@@ -16075,10 +16075,10 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="34"/>
-      <c r="C21" s="252" t="s">
+      <c r="C21" s="247" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="252"/>
+      <c r="D21" s="247"/>
       <c r="E21" s="246" t="s">
         <v>294</v>
       </c>
@@ -16099,10 +16099,10 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="188"/>
-      <c r="C22" s="248" t="s">
+      <c r="C22" s="249" t="s">
         <v>308</v>
       </c>
-      <c r="D22" s="249"/>
+      <c r="D22" s="250"/>
       <c r="E22" s="246" t="s">
         <v>182</v>
       </c>
@@ -16123,10 +16123,10 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="34"/>
-      <c r="C23" s="247" t="s">
+      <c r="C23" s="248" t="s">
         <v>134</v>
       </c>
-      <c r="D23" s="247"/>
+      <c r="D23" s="248"/>
       <c r="E23" s="209">
         <v>0.85</v>
       </c>
@@ -16149,10 +16149,10 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="34"/>
-      <c r="C24" s="247" t="s">
+      <c r="C24" s="248" t="s">
         <v>296</v>
       </c>
-      <c r="D24" s="247"/>
+      <c r="D24" s="248"/>
       <c r="E24" s="246" t="s">
         <v>182</v>
       </c>
@@ -16173,10 +16173,10 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="34"/>
-      <c r="C25" s="247" t="s">
+      <c r="C25" s="248" t="s">
         <v>133</v>
       </c>
-      <c r="D25" s="247"/>
+      <c r="D25" s="248"/>
       <c r="E25" s="209">
         <v>0.8</v>
       </c>
@@ -16215,38 +16215,16 @@
       <c r="D27" s="37"/>
       <c r="E27" s="37"/>
       <c r="F27" s="37"/>
-      <c r="G27" s="255" t="s">
+      <c r="G27" s="251" t="s">
         <v>167</v>
       </c>
-      <c r="H27" s="255"/>
-      <c r="I27" s="255"/>
-      <c r="J27" s="255"/>
-      <c r="K27" s="256"/>
+      <c r="H27" s="251"/>
+      <c r="I27" s="251"/>
+      <c r="J27" s="251"/>
+      <c r="K27" s="252"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
@@ -16257,6 +16235,28 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C8:D8" r:id="rId1" display="750g"/>
@@ -16326,8 +16326,8 @@
       <c r="C4" s="183"/>
       <c r="D4" s="183"/>
       <c r="E4" s="183"/>
-      <c r="F4" s="250"/>
-      <c r="G4" s="250"/>
+      <c r="F4" s="253"/>
+      <c r="G4" s="253"/>
       <c r="H4" s="183"/>
       <c r="I4" s="183"/>
       <c r="J4" s="189"/>
@@ -16345,27 +16345,27 @@
     </row>
     <row r="6" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="188"/>
-      <c r="C6" s="253" t="s">
+      <c r="C6" s="255" t="s">
         <v>257</v>
       </c>
-      <c r="D6" s="253"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="253"/>
-      <c r="G6" s="253"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="255"/>
       <c r="H6" s="177" t="s">
         <v>300</v>
       </c>
       <c r="I6" s="178" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J6" s="189"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="188"/>
-      <c r="C7" s="251" t="s">
-        <v>322</v>
-      </c>
-      <c r="D7" s="251"/>
+      <c r="C7" s="254" t="s">
+        <v>321</v>
+      </c>
+      <c r="D7" s="254"/>
       <c r="E7" s="136" t="s">
         <v>7</v>
       </c>
@@ -16385,10 +16385,10 @@
     </row>
     <row r="8" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="188"/>
-      <c r="C8" s="258" t="s">
+      <c r="C8" s="257" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="259"/>
+      <c r="D8" s="258"/>
       <c r="E8" s="208">
         <v>0.9</v>
       </c>
@@ -16408,10 +16408,10 @@
     </row>
     <row r="9" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="188"/>
-      <c r="C9" s="258" t="s">
+      <c r="C9" s="257" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="259"/>
+      <c r="D9" s="258"/>
       <c r="E9" s="208">
         <v>0.9</v>
       </c>
@@ -16431,10 +16431,10 @@
     </row>
     <row r="10" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="188"/>
-      <c r="C10" s="258" t="s">
-        <v>323</v>
-      </c>
-      <c r="D10" s="259"/>
+      <c r="C10" s="257" t="s">
+        <v>322</v>
+      </c>
+      <c r="D10" s="258"/>
       <c r="E10" s="208">
         <v>0.4</v>
       </c>
@@ -16454,10 +16454,10 @@
     </row>
     <row r="11" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="188"/>
-      <c r="C11" s="258" t="s">
+      <c r="C11" s="257" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="259"/>
+      <c r="D11" s="258"/>
       <c r="E11" s="208">
         <v>0.3</v>
       </c>
@@ -16477,10 +16477,10 @@
     </row>
     <row r="12" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="188"/>
-      <c r="C12" s="258" t="s">
+      <c r="C12" s="257" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="259"/>
+      <c r="D12" s="258"/>
       <c r="E12" s="208">
         <v>0.7</v>
       </c>
@@ -16500,10 +16500,10 @@
     </row>
     <row r="13" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="188"/>
-      <c r="C13" s="258" t="s">
+      <c r="C13" s="257" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="259"/>
+      <c r="D13" s="258"/>
       <c r="E13" s="211">
         <v>0.9</v>
       </c>
@@ -16523,14 +16523,14 @@
     </row>
     <row r="14" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="188"/>
-      <c r="C14" s="258" t="s">
-        <v>324</v>
-      </c>
-      <c r="D14" s="259"/>
-      <c r="E14" s="257" t="s">
+      <c r="C14" s="257" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" s="258"/>
+      <c r="E14" s="259" t="s">
         <v>182</v>
       </c>
-      <c r="F14" s="257"/>
+      <c r="F14" s="259"/>
       <c r="G14" s="180">
         <v>2500000</v>
       </c>
@@ -16544,10 +16544,10 @@
     </row>
     <row r="15" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="188"/>
-      <c r="C15" s="258" t="s">
+      <c r="C15" s="257" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="259"/>
+      <c r="D15" s="258"/>
       <c r="E15" s="208">
         <v>0.9</v>
       </c>
@@ -16567,10 +16567,10 @@
     </row>
     <row r="16" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="188"/>
-      <c r="C16" s="258" t="s">
+      <c r="C16" s="257" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="259"/>
+      <c r="D16" s="258"/>
       <c r="E16" s="208">
         <v>0.8</v>
       </c>
@@ -16590,10 +16590,10 @@
     </row>
     <row r="17" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="188"/>
-      <c r="C17" s="258" t="s">
+      <c r="C17" s="257" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="259"/>
+      <c r="D17" s="258"/>
       <c r="E17" s="208">
         <v>0.8</v>
       </c>
@@ -16627,16 +16627,22 @@
       <c r="C19" s="38"/>
       <c r="D19" s="191"/>
       <c r="E19" s="191"/>
-      <c r="F19" s="255" t="s">
+      <c r="F19" s="251" t="s">
         <v>167</v>
       </c>
-      <c r="G19" s="255"/>
-      <c r="H19" s="255"/>
-      <c r="I19" s="255"/>
-      <c r="J19" s="256"/>
+      <c r="G19" s="251"/>
+      <c r="H19" s="251"/>
+      <c r="I19" s="251"/>
+      <c r="J19" s="252"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="F19:J19"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
@@ -16646,12 +16652,6 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16789,44 +16789,44 @@
     </row>
     <row r="6" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="188"/>
-      <c r="C6" s="266" t="s">
+      <c r="C6" s="270" t="s">
         <v>287</v>
       </c>
-      <c r="D6" s="267"/>
-      <c r="E6" s="268" t="s">
+      <c r="D6" s="271"/>
+      <c r="E6" s="272" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="269"/>
-      <c r="G6" s="268" t="s">
+      <c r="F6" s="273"/>
+      <c r="G6" s="272" t="s">
         <v>286</v>
       </c>
-      <c r="H6" s="270"/>
+      <c r="H6" s="274"/>
       <c r="I6" s="183"/>
-      <c r="J6" s="266" t="s">
+      <c r="J6" s="270" t="s">
         <v>288</v>
       </c>
-      <c r="K6" s="267"/>
-      <c r="L6" s="264" t="s">
+      <c r="K6" s="271"/>
+      <c r="L6" s="268" t="s">
         <v>216</v>
       </c>
-      <c r="M6" s="265"/>
-      <c r="N6" s="268" t="s">
+      <c r="M6" s="269"/>
+      <c r="N6" s="272" t="s">
         <v>286</v>
       </c>
-      <c r="O6" s="270"/>
+      <c r="O6" s="274"/>
       <c r="P6" s="183"/>
-      <c r="Q6" s="266" t="s">
+      <c r="Q6" s="270" t="s">
         <v>289</v>
       </c>
-      <c r="R6" s="267"/>
-      <c r="S6" s="264" t="s">
+      <c r="R6" s="271"/>
+      <c r="S6" s="268" t="s">
         <v>216</v>
       </c>
-      <c r="T6" s="265"/>
-      <c r="U6" s="264" t="s">
+      <c r="T6" s="269"/>
+      <c r="U6" s="268" t="s">
         <v>286</v>
       </c>
-      <c r="V6" s="265"/>
+      <c r="V6" s="269"/>
       <c r="W6" s="189"/>
     </row>
     <row r="7" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -17189,14 +17189,14 @@
         <v>12321</v>
       </c>
       <c r="P14" s="183"/>
-      <c r="Q14" s="266" t="s">
+      <c r="Q14" s="270" t="s">
         <v>233</v>
       </c>
-      <c r="R14" s="267"/>
-      <c r="S14" s="264" t="s">
+      <c r="R14" s="271"/>
+      <c r="S14" s="268" t="s">
         <v>216</v>
       </c>
-      <c r="T14" s="265"/>
+      <c r="T14" s="269"/>
       <c r="U14" s="183"/>
       <c r="V14" s="183"/>
       <c r="W14" s="189"/>
@@ -17362,8 +17362,8 @@
       <c r="G19" s="183"/>
       <c r="H19" s="183"/>
       <c r="I19" s="183"/>
-      <c r="J19" s="271"/>
-      <c r="K19" s="272"/>
+      <c r="J19" s="264"/>
+      <c r="K19" s="265"/>
       <c r="L19" s="108" t="s">
         <v>139</v>
       </c>
@@ -17394,8 +17394,8 @@
       <c r="G20" s="183"/>
       <c r="H20" s="183"/>
       <c r="I20" s="183"/>
-      <c r="J20" s="273"/>
-      <c r="K20" s="274"/>
+      <c r="J20" s="266"/>
+      <c r="K20" s="267"/>
       <c r="L20" s="109" t="s">
         <v>181</v>
       </c>
@@ -17426,8 +17426,8 @@
       <c r="G21" s="183"/>
       <c r="H21" s="183"/>
       <c r="I21" s="183"/>
-      <c r="J21" s="271"/>
-      <c r="K21" s="272"/>
+      <c r="J21" s="264"/>
+      <c r="K21" s="265"/>
       <c r="L21" s="108" t="s">
         <v>139</v>
       </c>
@@ -17458,8 +17458,8 @@
       <c r="G22" s="183"/>
       <c r="H22" s="183"/>
       <c r="I22" s="183"/>
-      <c r="J22" s="273"/>
-      <c r="K22" s="274"/>
+      <c r="J22" s="266"/>
+      <c r="K22" s="267"/>
       <c r="L22" s="109" t="s">
         <v>181</v>
       </c>
@@ -17543,13 +17543,11 @@
     <row r="32" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="Q11:R12"/>
-    <mergeCell ref="J21:K22"/>
-    <mergeCell ref="J19:K20"/>
-    <mergeCell ref="J11:K12"/>
-    <mergeCell ref="J13:K14"/>
-    <mergeCell ref="Q15:R16"/>
-    <mergeCell ref="J17:K18"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="J15:K16"/>
+    <mergeCell ref="J9:K10"/>
     <mergeCell ref="U6:V6"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="S14:T14"/>
@@ -17566,11 +17564,13 @@
     <mergeCell ref="Q7:R8"/>
     <mergeCell ref="C11:D12"/>
     <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="C13:D14"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="J15:K16"/>
-    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="Q11:R12"/>
+    <mergeCell ref="J21:K22"/>
+    <mergeCell ref="J19:K20"/>
+    <mergeCell ref="J11:K12"/>
+    <mergeCell ref="J13:K14"/>
+    <mergeCell ref="Q15:R16"/>
+    <mergeCell ref="J17:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -17704,7 +17704,7 @@
       <c r="A9" s="197"/>
       <c r="B9" s="188"/>
       <c r="C9" s="202" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D9" s="203"/>
       <c r="E9" s="203"/>
@@ -17744,7 +17744,7 @@
       <c r="A12" s="197"/>
       <c r="B12" s="188"/>
       <c r="C12" s="202" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D12" s="203"/>
       <c r="E12" s="203"/>
@@ -17780,7 +17780,7 @@
       <c r="A15" s="197"/>
       <c r="B15" s="188"/>
       <c r="C15" s="202" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D15" s="203"/>
       <c r="E15" s="203"/>
@@ -17814,7 +17814,7 @@
       <c r="A18" s="197"/>
       <c r="B18" s="188"/>
       <c r="C18" s="202" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D18" s="203"/>
       <c r="E18" s="203"/>
@@ -17848,7 +17848,7 @@
       <c r="A21" s="197"/>
       <c r="B21" s="188"/>
       <c r="C21" s="202" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D21" s="203"/>
       <c r="E21" s="203"/>
@@ -17861,12 +17861,12 @@
       <c r="B22" s="190"/>
       <c r="C22" s="191"/>
       <c r="D22" s="191"/>
-      <c r="E22" s="255" t="s">
+      <c r="E22" s="251" t="s">
         <v>167</v>
       </c>
-      <c r="F22" s="255"/>
-      <c r="G22" s="255"/>
-      <c r="H22" s="256"/>
+      <c r="F22" s="251"/>
+      <c r="G22" s="251"/>
+      <c r="H22" s="252"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18013,50 +18013,50 @@
     </row>
     <row r="6" spans="2:23" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="34"/>
-      <c r="C6" s="266" t="s">
+      <c r="C6" s="270" t="s">
         <v>291</v>
       </c>
-      <c r="D6" s="267"/>
-      <c r="E6" s="268" t="s">
+      <c r="D6" s="271"/>
+      <c r="E6" s="272" t="s">
+        <v>319</v>
+      </c>
+      <c r="F6" s="273"/>
+      <c r="G6" s="272" t="s">
+        <v>316</v>
+      </c>
+      <c r="H6" s="274"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="270" t="s">
+        <v>292</v>
+      </c>
+      <c r="K6" s="271"/>
+      <c r="L6" s="277" t="s">
+        <v>217</v>
+      </c>
+      <c r="M6" s="278"/>
+      <c r="N6" s="272" t="s">
+        <v>316</v>
+      </c>
+      <c r="O6" s="274"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="270" t="s">
+        <v>260</v>
+      </c>
+      <c r="R6" s="271"/>
+      <c r="S6" s="268" t="s">
         <v>320</v>
       </c>
-      <c r="F6" s="269"/>
-      <c r="G6" s="268" t="s">
-        <v>317</v>
-      </c>
-      <c r="H6" s="270"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="266" t="s">
-        <v>292</v>
-      </c>
-      <c r="K6" s="267"/>
-      <c r="L6" s="275" t="s">
-        <v>217</v>
-      </c>
-      <c r="M6" s="276"/>
-      <c r="N6" s="268" t="s">
-        <v>317</v>
-      </c>
-      <c r="O6" s="270"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="266" t="s">
-        <v>260</v>
-      </c>
-      <c r="R6" s="267"/>
-      <c r="S6" s="264" t="s">
-        <v>321</v>
-      </c>
-      <c r="T6" s="265"/>
-      <c r="U6" s="268" t="s">
-        <v>317</v>
-      </c>
-      <c r="V6" s="270"/>
+      <c r="T6" s="269"/>
+      <c r="U6" s="272" t="s">
+        <v>316</v>
+      </c>
+      <c r="V6" s="274"/>
       <c r="W6" s="35"/>
     </row>
     <row r="7" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34"/>
       <c r="C7" s="260"/>
-      <c r="D7" s="281"/>
+      <c r="D7" s="275"/>
       <c r="E7" s="108" t="s">
         <v>139</v>
       </c>
@@ -18104,7 +18104,7 @@
     <row r="8" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="34"/>
       <c r="C8" s="262"/>
-      <c r="D8" s="282"/>
+      <c r="D8" s="276"/>
       <c r="E8" s="109" t="s">
         <v>181</v>
       </c>
@@ -18152,7 +18152,7 @@
     <row r="9" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="34"/>
       <c r="C9" s="260"/>
-      <c r="D9" s="281"/>
+      <c r="D9" s="275"/>
       <c r="E9" s="108" t="s">
         <v>139</v>
       </c>
@@ -18200,7 +18200,7 @@
     <row r="10" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="34"/>
       <c r="C10" s="262"/>
-      <c r="D10" s="282"/>
+      <c r="D10" s="276"/>
       <c r="E10" s="109" t="s">
         <v>181</v>
       </c>
@@ -18248,7 +18248,7 @@
     <row r="11" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="34"/>
       <c r="C11" s="260"/>
-      <c r="D11" s="281"/>
+      <c r="D11" s="275"/>
       <c r="E11" s="108" t="s">
         <v>139</v>
       </c>
@@ -18296,7 +18296,7 @@
     <row r="12" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="34"/>
       <c r="C12" s="262"/>
-      <c r="D12" s="282"/>
+      <c r="D12" s="276"/>
       <c r="E12" s="109" t="s">
         <v>181</v>
       </c>
@@ -18344,7 +18344,7 @@
     <row r="13" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="34"/>
       <c r="C13" s="260"/>
-      <c r="D13" s="281"/>
+      <c r="D13" s="275"/>
       <c r="E13" s="108" t="s">
         <v>139</v>
       </c>
@@ -18384,7 +18384,7 @@
     <row r="14" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="34"/>
       <c r="C14" s="262"/>
-      <c r="D14" s="282"/>
+      <c r="D14" s="276"/>
       <c r="E14" s="109" t="s">
         <v>181</v>
       </c>
@@ -18424,7 +18424,7 @@
     <row r="15" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="34"/>
       <c r="C15" s="260"/>
-      <c r="D15" s="281"/>
+      <c r="D15" s="275"/>
       <c r="E15" s="108" t="s">
         <v>139</v>
       </c>
@@ -18453,24 +18453,24 @@
         <v>1346</v>
       </c>
       <c r="P15" s="10"/>
-      <c r="Q15" s="266" t="s">
-        <v>318</v>
-      </c>
-      <c r="R15" s="267"/>
-      <c r="S15" s="264" t="s">
+      <c r="Q15" s="270" t="s">
+        <v>317</v>
+      </c>
+      <c r="R15" s="271"/>
+      <c r="S15" s="268" t="s">
         <v>293</v>
       </c>
-      <c r="T15" s="265"/>
-      <c r="U15" s="268" t="s">
-        <v>317</v>
-      </c>
-      <c r="V15" s="270"/>
+      <c r="T15" s="269"/>
+      <c r="U15" s="272" t="s">
+        <v>316</v>
+      </c>
+      <c r="V15" s="274"/>
       <c r="W15" s="35"/>
     </row>
     <row r="16" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="34"/>
       <c r="C16" s="262"/>
-      <c r="D16" s="282"/>
+      <c r="D16" s="276"/>
       <c r="E16" s="109" t="s">
         <v>181</v>
       </c>
@@ -18684,8 +18684,8 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="271"/>
-      <c r="K21" s="272"/>
+      <c r="J21" s="264"/>
+      <c r="K21" s="265"/>
       <c r="L21" s="108" t="s">
         <v>139</v>
       </c>
@@ -18724,8 +18724,8 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="273"/>
-      <c r="K22" s="274"/>
+      <c r="J22" s="266"/>
+      <c r="K22" s="267"/>
       <c r="L22" s="109" t="s">
         <v>181</v>
       </c>
@@ -18764,8 +18764,8 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="271"/>
-      <c r="K23" s="272"/>
+      <c r="J23" s="264"/>
+      <c r="K23" s="265"/>
       <c r="L23" s="108" t="s">
         <v>139</v>
       </c>
@@ -18804,8 +18804,8 @@
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="273"/>
-      <c r="K24" s="274"/>
+      <c r="J24" s="266"/>
+      <c r="K24" s="267"/>
       <c r="L24" s="109" t="s">
         <v>181</v>
       </c>
@@ -19075,8 +19075,8 @@
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
-      <c r="Q32" s="271"/>
-      <c r="R32" s="272"/>
+      <c r="Q32" s="264"/>
+      <c r="R32" s="265"/>
       <c r="S32" s="108" t="s">
         <v>139</v>
       </c>
@@ -19107,8 +19107,8 @@
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
-      <c r="Q33" s="273"/>
-      <c r="R33" s="274"/>
+      <c r="Q33" s="266"/>
+      <c r="R33" s="267"/>
       <c r="S33" s="109" t="s">
         <v>181</v>
       </c>
@@ -19340,11 +19340,11 @@
       <c r="W40" s="35"/>
     </row>
     <row r="41" spans="2:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="277" t="s">
-        <v>319</v>
-      </c>
-      <c r="C41" s="278"/>
-      <c r="D41" s="278"/>
+      <c r="B41" s="279" t="s">
+        <v>318</v>
+      </c>
+      <c r="C41" s="280"/>
+      <c r="D41" s="280"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -19366,44 +19366,49 @@
       <c r="W41" s="35"/>
     </row>
     <row r="42" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="279"/>
-      <c r="C42" s="280"/>
-      <c r="D42" s="280"/>
+      <c r="B42" s="281"/>
+      <c r="C42" s="282"/>
+      <c r="D42" s="282"/>
       <c r="E42" s="176"/>
       <c r="F42" s="176"/>
       <c r="G42" s="37"/>
       <c r="H42" s="37"/>
-      <c r="I42" s="255" t="s">
+      <c r="I42" s="251" t="s">
         <v>167</v>
       </c>
-      <c r="J42" s="255"/>
-      <c r="K42" s="255"/>
-      <c r="L42" s="255"/>
-      <c r="M42" s="255"/>
-      <c r="N42" s="255"/>
-      <c r="O42" s="255"/>
-      <c r="P42" s="255"/>
-      <c r="Q42" s="255"/>
-      <c r="R42" s="255"/>
-      <c r="S42" s="255"/>
-      <c r="T42" s="255"/>
-      <c r="U42" s="255"/>
-      <c r="V42" s="255"/>
-      <c r="W42" s="256"/>
+      <c r="J42" s="251"/>
+      <c r="K42" s="251"/>
+      <c r="L42" s="251"/>
+      <c r="M42" s="251"/>
+      <c r="N42" s="251"/>
+      <c r="O42" s="251"/>
+      <c r="P42" s="251"/>
+      <c r="Q42" s="251"/>
+      <c r="R42" s="251"/>
+      <c r="S42" s="251"/>
+      <c r="T42" s="251"/>
+      <c r="U42" s="251"/>
+      <c r="V42" s="251"/>
+      <c r="W42" s="252"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D8"/>
-    <mergeCell ref="J7:K8"/>
-    <mergeCell ref="J13:K14"/>
-    <mergeCell ref="J11:K12"/>
-    <mergeCell ref="J15:K16"/>
-    <mergeCell ref="C15:D16"/>
-    <mergeCell ref="C9:D10"/>
-    <mergeCell ref="J9:K10"/>
-    <mergeCell ref="C11:D12"/>
-    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="I42:W42"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="B41:D42"/>
+    <mergeCell ref="Q7:R8"/>
+    <mergeCell ref="Q9:R10"/>
+    <mergeCell ref="Q11:R12"/>
     <mergeCell ref="Q30:R31"/>
     <mergeCell ref="Q16:R17"/>
     <mergeCell ref="Q38:R39"/>
@@ -19420,22 +19425,17 @@
     <mergeCell ref="Q26:R27"/>
     <mergeCell ref="Q18:R19"/>
     <mergeCell ref="J17:K18"/>
-    <mergeCell ref="I42:W42"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="S15:T15"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="B41:D42"/>
-    <mergeCell ref="Q7:R8"/>
-    <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="Q11:R12"/>
+    <mergeCell ref="J15:K16"/>
+    <mergeCell ref="C15:D16"/>
+    <mergeCell ref="C9:D10"/>
+    <mergeCell ref="J9:K10"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C13:D14"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D8"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="J13:K14"/>
+    <mergeCell ref="J11:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20014,13 +20014,13 @@
     <row r="5" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="34"/>
       <c r="C5" s="122" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D5" s="114" t="s">
         <v>300</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F5" s="35"/>
     </row>
@@ -20182,11 +20182,11 @@
         <v>303</v>
       </c>
       <c r="C19" s="38"/>
-      <c r="D19" s="255" t="s">
+      <c r="D19" s="251" t="s">
         <v>215</v>
       </c>
-      <c r="E19" s="255"/>
-      <c r="F19" s="256"/>
+      <c r="E19" s="251"/>
+      <c r="F19" s="252"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -20291,8 +20291,8 @@
     </row>
     <row r="8" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="34"/>
-      <c r="C8" s="293"/>
-      <c r="D8" s="302" t="s">
+      <c r="C8" s="286"/>
+      <c r="D8" s="295" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="160" t="s">
@@ -20301,43 +20301,43 @@
       <c r="F8" s="161">
         <v>42500000</v>
       </c>
-      <c r="G8" s="290">
+      <c r="G8" s="283">
         <v>12</v>
       </c>
       <c r="H8" s="35"/>
     </row>
     <row r="9" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="34"/>
-      <c r="C9" s="294"/>
-      <c r="D9" s="303"/>
+      <c r="C9" s="287"/>
+      <c r="D9" s="296"/>
       <c r="E9" s="162" t="s">
         <v>115</v>
       </c>
       <c r="F9" s="162">
         <v>50500000</v>
       </c>
-      <c r="G9" s="291"/>
+      <c r="G9" s="284"/>
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="188"/>
-      <c r="C10" s="294"/>
-      <c r="D10" s="303"/>
+      <c r="C10" s="287"/>
+      <c r="D10" s="296"/>
       <c r="E10" s="163" t="s">
         <v>116</v>
       </c>
       <c r="F10" s="163">
         <v>3500000</v>
       </c>
-      <c r="G10" s="292"/>
+      <c r="G10" s="285"/>
       <c r="H10" s="189"/>
     </row>
     <row r="11" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="34"/>
-      <c r="C11" s="294"/>
-      <c r="D11" s="304"/>
+      <c r="C11" s="287"/>
+      <c r="D11" s="297"/>
       <c r="E11" s="163" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F11" s="163">
         <v>13000000</v>
@@ -20349,7 +20349,7 @@
     </row>
     <row r="12" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="34"/>
-      <c r="C12" s="294"/>
+      <c r="C12" s="287"/>
       <c r="D12" s="120" t="s">
         <v>29</v>
       </c>
@@ -20367,8 +20367,8 @@
     </row>
     <row r="13" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="34"/>
-      <c r="C13" s="294"/>
-      <c r="D13" s="283" t="s">
+      <c r="C13" s="287"/>
+      <c r="D13" s="298" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="142" t="s">
@@ -20377,28 +20377,28 @@
       <c r="F13" s="142">
         <v>35500000</v>
       </c>
-      <c r="G13" s="284">
+      <c r="G13" s="299">
         <v>14</v>
       </c>
       <c r="H13" s="35"/>
     </row>
     <row r="14" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="34"/>
-      <c r="C14" s="294"/>
-      <c r="D14" s="283"/>
+      <c r="C14" s="287"/>
+      <c r="D14" s="298"/>
       <c r="E14" s="143" t="s">
         <v>249</v>
       </c>
       <c r="F14" s="143">
         <v>16500000</v>
       </c>
-      <c r="G14" s="284"/>
+      <c r="G14" s="299"/>
       <c r="H14" s="35"/>
     </row>
     <row r="15" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="34"/>
-      <c r="C15" s="294"/>
-      <c r="D15" s="285" t="s">
+      <c r="C15" s="287"/>
+      <c r="D15" s="300" t="s">
         <v>147</v>
       </c>
       <c r="E15" s="144" t="s">
@@ -20414,8 +20414,8 @@
     </row>
     <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34"/>
-      <c r="C16" s="295"/>
-      <c r="D16" s="285"/>
+      <c r="C16" s="288"/>
+      <c r="D16" s="300"/>
       <c r="E16" s="145" t="s">
         <v>250</v>
       </c>
@@ -20439,7 +20439,7 @@
     <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="34"/>
       <c r="C18" s="158"/>
-      <c r="D18" s="286" t="s">
+      <c r="D18" s="301" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="164" t="s">
@@ -20448,7 +20448,7 @@
       <c r="F18" s="161">
         <v>260000000</v>
       </c>
-      <c r="G18" s="296">
+      <c r="G18" s="289">
         <v>10</v>
       </c>
       <c r="H18" s="35"/>
@@ -20456,40 +20456,40 @@
     <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="34"/>
       <c r="C19" s="159"/>
-      <c r="D19" s="287"/>
+      <c r="D19" s="302"/>
       <c r="E19" s="165" t="s">
         <v>114</v>
       </c>
       <c r="F19" s="162">
         <v>12000000</v>
       </c>
-      <c r="G19" s="297"/>
+      <c r="G19" s="290"/>
       <c r="H19" s="35"/>
     </row>
     <row r="20" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="34"/>
       <c r="C20" s="156"/>
-      <c r="D20" s="287"/>
+      <c r="D20" s="302"/>
       <c r="E20" s="165" t="s">
         <v>115</v>
       </c>
       <c r="F20" s="162">
         <v>4000000</v>
       </c>
-      <c r="G20" s="297"/>
+      <c r="G20" s="290"/>
       <c r="H20" s="35"/>
     </row>
     <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="34"/>
       <c r="C21" s="168"/>
-      <c r="D21" s="288"/>
+      <c r="D21" s="303"/>
       <c r="E21" s="166" t="s">
         <v>116</v>
       </c>
       <c r="F21" s="163">
         <v>800000</v>
       </c>
-      <c r="G21" s="297"/>
+      <c r="G21" s="290"/>
       <c r="H21" s="35"/>
     </row>
     <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -20504,7 +20504,7 @@
       <c r="F22" s="163">
         <v>30000000</v>
       </c>
-      <c r="G22" s="298"/>
+      <c r="G22" s="291"/>
       <c r="H22" s="35"/>
     </row>
     <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -20535,8 +20535,8 @@
     </row>
     <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="34"/>
-      <c r="C25" s="301"/>
-      <c r="D25" s="285" t="s">
+      <c r="C25" s="294"/>
+      <c r="D25" s="300" t="s">
         <v>27</v>
       </c>
       <c r="E25" s="142" t="s">
@@ -20545,87 +20545,87 @@
       <c r="F25" s="142">
         <v>32500000</v>
       </c>
-      <c r="G25" s="300">
+      <c r="G25" s="293">
         <v>8</v>
       </c>
       <c r="H25" s="35"/>
     </row>
     <row r="26" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="34"/>
-      <c r="C26" s="301"/>
-      <c r="D26" s="285"/>
+      <c r="C26" s="294"/>
+      <c r="D26" s="300"/>
       <c r="E26" s="148" t="s">
         <v>115</v>
       </c>
       <c r="F26" s="149">
         <v>13000000</v>
       </c>
-      <c r="G26" s="300"/>
+      <c r="G26" s="293"/>
       <c r="H26" s="35"/>
     </row>
     <row r="27" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="34"/>
-      <c r="C27" s="301"/>
-      <c r="D27" s="285"/>
+      <c r="C27" s="294"/>
+      <c r="D27" s="300"/>
       <c r="E27" s="148" t="s">
         <v>116</v>
       </c>
       <c r="F27" s="149">
         <v>12500000</v>
       </c>
-      <c r="G27" s="300"/>
+      <c r="G27" s="293"/>
       <c r="H27" s="35"/>
     </row>
     <row r="28" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="34"/>
-      <c r="C28" s="301"/>
-      <c r="D28" s="285"/>
+      <c r="C28" s="294"/>
+      <c r="D28" s="300"/>
       <c r="E28" s="148" t="s">
         <v>119</v>
       </c>
       <c r="F28" s="149">
         <v>4000000</v>
       </c>
-      <c r="G28" s="300"/>
+      <c r="G28" s="293"/>
       <c r="H28" s="35"/>
     </row>
     <row r="29" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="34"/>
-      <c r="C29" s="301"/>
-      <c r="D29" s="285"/>
+      <c r="C29" s="294"/>
+      <c r="D29" s="300"/>
       <c r="E29" s="150" t="s">
         <v>117</v>
       </c>
       <c r="F29" s="143">
         <v>15000000</v>
       </c>
-      <c r="G29" s="300"/>
+      <c r="G29" s="293"/>
       <c r="H29" s="35"/>
     </row>
     <row r="30" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="34"/>
-      <c r="C30" s="301"/>
-      <c r="D30" s="285" t="s">
+      <c r="C30" s="294"/>
+      <c r="D30" s="300" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="289" t="s">
+      <c r="E30" s="304" t="s">
         <v>120</v>
       </c>
-      <c r="F30" s="299">
+      <c r="F30" s="292">
         <v>77000000</v>
       </c>
-      <c r="G30" s="300">
+      <c r="G30" s="293">
         <v>12</v>
       </c>
       <c r="H30" s="35"/>
     </row>
     <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="34"/>
-      <c r="C31" s="301"/>
-      <c r="D31" s="285"/>
-      <c r="E31" s="289"/>
-      <c r="F31" s="299"/>
-      <c r="G31" s="300"/>
+      <c r="C31" s="294"/>
+      <c r="D31" s="300"/>
+      <c r="E31" s="304"/>
+      <c r="F31" s="292"/>
+      <c r="G31" s="293"/>
       <c r="H31" s="35"/>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -20639,8 +20639,8 @@
     </row>
     <row r="33" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="34"/>
-      <c r="C33" s="293"/>
-      <c r="D33" s="286" t="s">
+      <c r="C33" s="286"/>
+      <c r="D33" s="301" t="s">
         <v>27</v>
       </c>
       <c r="E33" s="167" t="s">
@@ -20649,61 +20649,61 @@
       <c r="F33" s="142">
         <v>18000000</v>
       </c>
-      <c r="G33" s="296">
+      <c r="G33" s="289">
         <v>5</v>
       </c>
       <c r="H33" s="35"/>
     </row>
     <row r="34" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="34"/>
-      <c r="C34" s="294"/>
-      <c r="D34" s="287"/>
+      <c r="C34" s="287"/>
+      <c r="D34" s="302"/>
       <c r="E34" s="165" t="s">
         <v>115</v>
       </c>
       <c r="F34" s="149">
         <v>20000000</v>
       </c>
-      <c r="G34" s="297"/>
+      <c r="G34" s="290"/>
       <c r="H34" s="35"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="34"/>
-      <c r="C35" s="294"/>
-      <c r="D35" s="287"/>
+      <c r="C35" s="287"/>
+      <c r="D35" s="302"/>
       <c r="E35" s="165" t="s">
         <v>116</v>
       </c>
       <c r="F35" s="149">
         <v>1800000</v>
       </c>
-      <c r="G35" s="297"/>
+      <c r="G35" s="290"/>
       <c r="H35" s="35"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="34"/>
-      <c r="C36" s="294"/>
-      <c r="D36" s="287"/>
+      <c r="C36" s="287"/>
+      <c r="D36" s="302"/>
       <c r="E36" s="165" t="s">
         <v>114</v>
       </c>
       <c r="F36" s="149">
         <v>26500000</v>
       </c>
-      <c r="G36" s="297"/>
+      <c r="G36" s="290"/>
       <c r="H36" s="35"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="34"/>
-      <c r="C37" s="295"/>
-      <c r="D37" s="288"/>
+      <c r="C37" s="288"/>
+      <c r="D37" s="303"/>
       <c r="E37" s="166" t="s">
         <v>117</v>
       </c>
       <c r="F37" s="143">
         <v>4500000</v>
       </c>
-      <c r="G37" s="298"/>
+      <c r="G37" s="291"/>
       <c r="H37" s="35"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -20719,15 +20719,24 @@
       <c r="B39" s="36"/>
       <c r="C39" s="38"/>
       <c r="D39" s="41"/>
-      <c r="E39" s="255" t="s">
+      <c r="E39" s="251" t="s">
         <v>215</v>
       </c>
-      <c r="F39" s="255"/>
-      <c r="G39" s="255"/>
-      <c r="H39" s="256"/>
+      <c r="F39" s="251"/>
+      <c r="G39" s="251"/>
+      <c r="H39" s="252"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D33:D37"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
     <mergeCell ref="G8:G10"/>
     <mergeCell ref="C33:C37"/>
     <mergeCell ref="G33:G37"/>
@@ -20738,15 +20747,6 @@
     <mergeCell ref="C25:C31"/>
     <mergeCell ref="C8:C16"/>
     <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D33:D37"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D25:D29"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="90" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>